<commit_message>
Working on hybrid MPI OMP graphs
</commit_message>
<xml_diff>
--- a/project-2/results/spreadsheet/openmpi.xlsx
+++ b/project-2/results/spreadsheet/openmpi.xlsx
@@ -7,11 +7,11 @@
     <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="openmpi" sheetId="1" r:id="rId1"/>
-    <sheet name="1cpu" sheetId="5" r:id="rId2"/>
-    <sheet name="2cpu" sheetId="2" r:id="rId3"/>
-    <sheet name="4cpu" sheetId="3" r:id="rId4"/>
-    <sheet name="8cpu" sheetId="4" r:id="rId5"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="1core" sheetId="5" r:id="rId2"/>
+    <sheet name="2cores" sheetId="2" r:id="rId3"/>
+    <sheet name="4cores" sheetId="3" r:id="rId4"/>
+    <sheet name="8cores" sheetId="4" r:id="rId5"/>
     <sheet name="Conclusions" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -762,6 +762,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -775,7 +776,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'1cpu'!$F$1</c:f>
+              <c:f>'1core'!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -786,7 +787,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'1cpu'!$E$2:$E$9</c:f>
+              <c:f>'1core'!$E$2:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -819,7 +820,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'1cpu'!$F$2:$F$9</c:f>
+              <c:f>'1core'!$F$2:$F$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -860,11 +861,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="213172224"/>
-        <c:axId val="213172800"/>
+        <c:axId val="212910080"/>
+        <c:axId val="212910656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="213172224"/>
+        <c:axId val="212910080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="32"/>
@@ -888,18 +889,19 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="213172800"/>
+        <c:crossAx val="212910656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="213172800"/>
+        <c:axId val="212910656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="18"/>
@@ -923,13 +925,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="213172224"/>
+        <c:crossAx val="212910080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -981,7 +984,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1020,7 +1022,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'2cpu'!$E$2</c:f>
+              <c:f>'2cores'!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1031,7 +1033,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'2cpu'!$D$3:$D$10</c:f>
+              <c:f>'2cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1064,7 +1066,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2cpu'!$E$3:$E$10</c:f>
+              <c:f>'2cores'!$E$3:$E$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1102,7 +1104,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'2cpu'!$F$2</c:f>
+              <c:f>'2cores'!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1113,7 +1115,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'2cpu'!$D$3:$D$10</c:f>
+              <c:f>'2cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1146,7 +1148,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2cpu'!$F$3:$F$10</c:f>
+              <c:f>'2cores'!$F$3:$F$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1184,7 +1186,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'2cpu'!$G$2</c:f>
+              <c:f>'2cores'!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1195,7 +1197,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'2cpu'!$D$3:$D$10</c:f>
+              <c:f>'2cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1228,7 +1230,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2cpu'!$G$3:$G$10</c:f>
+              <c:f>'2cores'!$G$3:$G$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1266,7 +1268,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'2cpu'!$H$2</c:f>
+              <c:f>'2cores'!$H$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1277,7 +1279,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'2cpu'!$D$3:$D$10</c:f>
+              <c:f>'2cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1310,7 +1312,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2cpu'!$H$3:$H$10</c:f>
+              <c:f>'2cores'!$H$3:$H$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1348,7 +1350,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'2cpu'!$I$2</c:f>
+              <c:f>'2cores'!$I$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1359,7 +1361,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'2cpu'!$D$3:$D$10</c:f>
+              <c:f>'2cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1392,7 +1394,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2cpu'!$I$3:$I$10</c:f>
+              <c:f>'2cores'!$I$3:$I$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1430,7 +1432,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'2cpu'!$J$2</c:f>
+              <c:f>'2cores'!$J$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1441,7 +1443,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'2cpu'!$D$3:$D$10</c:f>
+              <c:f>'2cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1474,7 +1476,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2cpu'!$J$3:$J$10</c:f>
+              <c:f>'2cores'!$J$3:$J$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1512,7 +1514,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>'2cpu'!$K$2</c:f>
+              <c:f>'2cores'!$K$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1523,7 +1525,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'2cpu'!$D$3:$D$10</c:f>
+              <c:f>'2cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1556,7 +1558,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2cpu'!$K$3:$K$10</c:f>
+              <c:f>'2cores'!$K$3:$K$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1597,12 +1599,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="214269952"/>
-        <c:axId val="213174528"/>
-        <c:axId val="213198080"/>
+        <c:axId val="213980160"/>
+        <c:axId val="212912384"/>
+        <c:axId val="212935936"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="214269952"/>
+        <c:axId val="213980160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1638,7 +1640,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="213174528"/>
+        <c:crossAx val="212912384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1646,7 +1648,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="213174528"/>
+        <c:axId val="212912384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1683,12 +1685,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="214269952"/>
+        <c:crossAx val="213980160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="213198080"/>
+        <c:axId val="212935936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1723,7 +1725,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="213174528"/>
+        <c:crossAx val="212912384"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -1774,7 +1776,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1798,7 +1799,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'2cpu'!$E$2</c:f>
+              <c:f>'2cores'!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1809,7 +1810,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'2cpu'!$D$3:$D$10</c:f>
+              <c:f>'2cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1842,7 +1843,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'2cpu'!$E$3:$E$10</c:f>
+              <c:f>'2cores'!$E$3:$E$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1880,7 +1881,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'2cpu'!$F$2</c:f>
+              <c:f>'2cores'!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1891,7 +1892,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'2cpu'!$D$3:$D$10</c:f>
+              <c:f>'2cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1924,7 +1925,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'2cpu'!$F$3:$F$10</c:f>
+              <c:f>'2cores'!$F$3:$F$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1962,7 +1963,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'2cpu'!$G$2</c:f>
+              <c:f>'2cores'!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1973,7 +1974,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'2cpu'!$D$3:$D$10</c:f>
+              <c:f>'2cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2006,7 +2007,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'2cpu'!$G$3:$G$10</c:f>
+              <c:f>'2cores'!$G$3:$G$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2044,7 +2045,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'2cpu'!$H$2</c:f>
+              <c:f>'2cores'!$H$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2055,7 +2056,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'2cpu'!$D$3:$D$10</c:f>
+              <c:f>'2cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2088,7 +2089,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'2cpu'!$H$3:$H$10</c:f>
+              <c:f>'2cores'!$H$3:$H$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2126,7 +2127,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'2cpu'!$I$2</c:f>
+              <c:f>'2cores'!$I$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2137,7 +2138,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'2cpu'!$D$3:$D$10</c:f>
+              <c:f>'2cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2170,7 +2171,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'2cpu'!$I$3:$I$10</c:f>
+              <c:f>'2cores'!$I$3:$I$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2208,7 +2209,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'2cpu'!$J$2</c:f>
+              <c:f>'2cores'!$J$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2219,7 +2220,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'2cpu'!$D$3:$D$10</c:f>
+              <c:f>'2cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2252,7 +2253,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'2cpu'!$J$3:$J$10</c:f>
+              <c:f>'2cores'!$J$3:$J$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2290,7 +2291,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>'2cpu'!$K$2</c:f>
+              <c:f>'2cores'!$K$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2301,7 +2302,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'2cpu'!$D$3:$D$10</c:f>
+              <c:f>'2cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2334,7 +2335,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'2cpu'!$K$3:$K$10</c:f>
+              <c:f>'2cores'!$K$3:$K$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2375,11 +2376,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="222076224"/>
-        <c:axId val="222073344"/>
+        <c:axId val="212914688"/>
+        <c:axId val="212915264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="222076224"/>
+        <c:axId val="212914688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="32"/>
@@ -2417,12 +2418,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="222073344"/>
+        <c:crossAx val="212915264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="222073344"/>
+        <c:axId val="212915264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2459,7 +2460,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="222076224"/>
+        <c:crossAx val="212914688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2511,7 +2512,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2550,7 +2550,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'4cpu'!$E$2</c:f>
+              <c:f>'4cores'!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2561,7 +2561,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'4cpu'!$D$3:$D$10</c:f>
+              <c:f>'4cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2594,7 +2594,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'4cpu'!$E$3:$E$10</c:f>
+              <c:f>'4cores'!$E$3:$E$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2632,7 +2632,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'4cpu'!$F$2</c:f>
+              <c:f>'4cores'!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2643,7 +2643,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'4cpu'!$D$3:$D$10</c:f>
+              <c:f>'4cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2676,7 +2676,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'4cpu'!$F$3:$F$10</c:f>
+              <c:f>'4cores'!$F$3:$F$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2714,7 +2714,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'4cpu'!$G$2</c:f>
+              <c:f>'4cores'!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2725,7 +2725,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'4cpu'!$D$3:$D$10</c:f>
+              <c:f>'4cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2758,7 +2758,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'4cpu'!$G$3:$G$10</c:f>
+              <c:f>'4cores'!$G$3:$G$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2796,7 +2796,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'4cpu'!$H$2</c:f>
+              <c:f>'4cores'!$H$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2807,7 +2807,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'4cpu'!$D$3:$D$10</c:f>
+              <c:f>'4cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2840,7 +2840,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'4cpu'!$H$3:$H$10</c:f>
+              <c:f>'4cores'!$H$3:$H$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2878,7 +2878,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'4cpu'!$I$2</c:f>
+              <c:f>'4cores'!$I$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2889,7 +2889,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'4cpu'!$D$3:$D$10</c:f>
+              <c:f>'4cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2922,7 +2922,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'4cpu'!$I$3:$I$10</c:f>
+              <c:f>'4cores'!$I$3:$I$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2960,7 +2960,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'4cpu'!$J$2</c:f>
+              <c:f>'4cores'!$J$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2971,7 +2971,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'4cpu'!$D$3:$D$10</c:f>
+              <c:f>'4cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3004,7 +3004,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'4cpu'!$J$3:$J$10</c:f>
+              <c:f>'4cores'!$J$3:$J$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3042,7 +3042,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>'4cpu'!$K$2</c:f>
+              <c:f>'4cores'!$K$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3053,7 +3053,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'4cpu'!$D$3:$D$10</c:f>
+              <c:f>'4cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3086,7 +3086,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'4cpu'!$K$3:$K$10</c:f>
+              <c:f>'4cores'!$K$3:$K$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3124,7 +3124,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>'4cpu'!$L$2</c:f>
+              <c:f>'4cores'!$L$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3135,7 +3135,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'4cpu'!$D$3:$D$10</c:f>
+              <c:f>'4cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3168,7 +3168,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'4cpu'!$L$3:$L$10</c:f>
+              <c:f>'4cores'!$L$3:$L$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3206,7 +3206,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>'4cpu'!$M$2</c:f>
+              <c:f>'4cores'!$M$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3222,7 +3222,7 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'4cpu'!$D$3:$D$10</c:f>
+              <c:f>'4cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3255,7 +3255,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'4cpu'!$M$3:$M$10</c:f>
+              <c:f>'4cores'!$M$3:$M$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3293,7 +3293,7 @@
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>'4cpu'!$N$2</c:f>
+              <c:f>'4cores'!$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3309,7 +3309,7 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'4cpu'!$D$3:$D$10</c:f>
+              <c:f>'4cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3342,7 +3342,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'4cpu'!$N$3:$N$10</c:f>
+              <c:f>'4cores'!$N$3:$N$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3380,7 +3380,7 @@
           <c:order val="10"/>
           <c:tx>
             <c:strRef>
-              <c:f>'4cpu'!$O$2</c:f>
+              <c:f>'4cores'!$O$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3396,7 +3396,7 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'4cpu'!$D$3:$D$10</c:f>
+              <c:f>'4cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3429,7 +3429,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'4cpu'!$O$3:$O$10</c:f>
+              <c:f>'4cores'!$O$3:$O$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3467,7 +3467,7 @@
           <c:order val="11"/>
           <c:tx>
             <c:strRef>
-              <c:f>'4cpu'!$P$2</c:f>
+              <c:f>'4cores'!$P$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3483,7 +3483,7 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'4cpu'!$D$3:$D$10</c:f>
+              <c:f>'4cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3516,7 +3516,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'4cpu'!$P$3:$P$10</c:f>
+              <c:f>'4cores'!$P$3:$P$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3554,7 +3554,7 @@
           <c:order val="12"/>
           <c:tx>
             <c:strRef>
-              <c:f>'4cpu'!$Q$2</c:f>
+              <c:f>'4cores'!$Q$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3570,7 +3570,7 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'4cpu'!$D$3:$D$10</c:f>
+              <c:f>'4cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3603,7 +3603,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'4cpu'!$Q$3:$Q$10</c:f>
+              <c:f>'4cores'!$Q$3:$Q$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3644,12 +3644,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="214273024"/>
-        <c:axId val="213176832"/>
-        <c:axId val="213199360"/>
+        <c:axId val="214294528"/>
+        <c:axId val="212917568"/>
+        <c:axId val="212937216"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="214273024"/>
+        <c:axId val="214294528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3685,7 +3685,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="213176832"/>
+        <c:crossAx val="212917568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3693,7 +3693,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="213176832"/>
+        <c:axId val="212917568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3730,12 +3730,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="214273024"/>
+        <c:crossAx val="214294528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="213199360"/>
+        <c:axId val="212937216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3770,7 +3770,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="213176832"/>
+        <c:crossAx val="212917568"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -3821,7 +3821,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3845,7 +3844,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'4cpu'!$E$2</c:f>
+              <c:f>'4cores'!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3856,7 +3855,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'4cpu'!$D$3:$D$10</c:f>
+              <c:f>'4cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3889,7 +3888,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'4cpu'!$E$3:$E$10</c:f>
+              <c:f>'4cores'!$E$3:$E$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3927,7 +3926,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'4cpu'!$F$2</c:f>
+              <c:f>'4cores'!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3938,7 +3937,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'4cpu'!$D$3:$D$10</c:f>
+              <c:f>'4cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3971,7 +3970,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'4cpu'!$F$3:$F$10</c:f>
+              <c:f>'4cores'!$F$3:$F$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4009,7 +4008,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'4cpu'!$G$2</c:f>
+              <c:f>'4cores'!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4020,7 +4019,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'4cpu'!$D$3:$D$10</c:f>
+              <c:f>'4cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4053,7 +4052,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'4cpu'!$G$3:$G$10</c:f>
+              <c:f>'4cores'!$G$3:$G$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4091,7 +4090,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'4cpu'!$H$2</c:f>
+              <c:f>'4cores'!$H$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4102,7 +4101,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'4cpu'!$D$3:$D$10</c:f>
+              <c:f>'4cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4135,7 +4134,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'4cpu'!$H$3:$H$10</c:f>
+              <c:f>'4cores'!$H$3:$H$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4173,7 +4172,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'4cpu'!$I$2</c:f>
+              <c:f>'4cores'!$I$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4184,7 +4183,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'4cpu'!$D$3:$D$10</c:f>
+              <c:f>'4cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4217,7 +4216,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'4cpu'!$I$3:$I$10</c:f>
+              <c:f>'4cores'!$I$3:$I$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4255,7 +4254,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'4cpu'!$J$2</c:f>
+              <c:f>'4cores'!$J$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4266,7 +4265,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'4cpu'!$D$3:$D$10</c:f>
+              <c:f>'4cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4299,7 +4298,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'4cpu'!$J$3:$J$10</c:f>
+              <c:f>'4cores'!$J$3:$J$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4337,7 +4336,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>'4cpu'!$K$2</c:f>
+              <c:f>'4cores'!$K$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4348,7 +4347,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'4cpu'!$D$3:$D$10</c:f>
+              <c:f>'4cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4381,7 +4380,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'4cpu'!$K$3:$K$10</c:f>
+              <c:f>'4cores'!$K$3:$K$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4419,7 +4418,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>'4cpu'!$L$2</c:f>
+              <c:f>'4cores'!$L$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4430,7 +4429,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'4cpu'!$D$3:$D$10</c:f>
+              <c:f>'4cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4463,7 +4462,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'4cpu'!$L$3:$L$10</c:f>
+              <c:f>'4cores'!$L$3:$L$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4501,7 +4500,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>'4cpu'!$M$2</c:f>
+              <c:f>'4cores'!$M$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4512,7 +4511,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'4cpu'!$D$3:$D$10</c:f>
+              <c:f>'4cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4545,7 +4544,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'4cpu'!$M$3:$M$10</c:f>
+              <c:f>'4cores'!$M$3:$M$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4583,7 +4582,7 @@
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>'4cpu'!$N$2</c:f>
+              <c:f>'4cores'!$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4594,7 +4593,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'4cpu'!$D$3:$D$10</c:f>
+              <c:f>'4cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4627,7 +4626,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'4cpu'!$N$3:$N$10</c:f>
+              <c:f>'4cores'!$N$3:$N$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4665,7 +4664,7 @@
           <c:order val="10"/>
           <c:tx>
             <c:strRef>
-              <c:f>'4cpu'!$O$2</c:f>
+              <c:f>'4cores'!$O$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4676,7 +4675,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'4cpu'!$D$3:$D$10</c:f>
+              <c:f>'4cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4709,7 +4708,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'4cpu'!$O$3:$O$10</c:f>
+              <c:f>'4cores'!$O$3:$O$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4747,7 +4746,7 @@
           <c:order val="11"/>
           <c:tx>
             <c:strRef>
-              <c:f>'4cpu'!$P$2</c:f>
+              <c:f>'4cores'!$P$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4758,7 +4757,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'4cpu'!$D$3:$D$10</c:f>
+              <c:f>'4cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4791,7 +4790,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'4cpu'!$P$3:$P$10</c:f>
+              <c:f>'4cores'!$P$3:$P$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4829,7 +4828,7 @@
           <c:order val="12"/>
           <c:tx>
             <c:strRef>
-              <c:f>'4cpu'!$Q$2</c:f>
+              <c:f>'4cores'!$Q$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4840,7 +4839,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'4cpu'!$D$3:$D$10</c:f>
+              <c:f>'4cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4873,7 +4872,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'4cpu'!$Q$3:$Q$10</c:f>
+              <c:f>'4cores'!$Q$3:$Q$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4914,11 +4913,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="91652672"/>
-        <c:axId val="222070464"/>
+        <c:axId val="214166336"/>
+        <c:axId val="214166912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91652672"/>
+        <c:axId val="214166336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="32"/>
@@ -4956,12 +4955,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="222070464"/>
+        <c:crossAx val="214166912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="222070464"/>
+        <c:axId val="214166912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="47"/>
@@ -5000,7 +4999,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91652672"/>
+        <c:crossAx val="214166336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5052,7 +5051,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5091,7 +5089,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$E$2</c:f>
+              <c:f>'8cores'!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5102,7 +5100,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -5135,7 +5133,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'8cpu'!$E$3:$E$10</c:f>
+              <c:f>'8cores'!$E$3:$E$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -5173,7 +5171,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$F$2</c:f>
+              <c:f>'8cores'!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5184,7 +5182,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -5217,7 +5215,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'8cpu'!$F$3:$F$10</c:f>
+              <c:f>'8cores'!$F$3:$F$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -5255,7 +5253,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$G$2</c:f>
+              <c:f>'8cores'!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5266,7 +5264,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -5299,7 +5297,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'8cpu'!$G$3:$G$10</c:f>
+              <c:f>'8cores'!$G$3:$G$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -5337,7 +5335,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$H$2</c:f>
+              <c:f>'8cores'!$H$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5348,7 +5346,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -5381,7 +5379,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'8cpu'!$H$3:$H$10</c:f>
+              <c:f>'8cores'!$H$3:$H$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -5419,7 +5417,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$I$2</c:f>
+              <c:f>'8cores'!$I$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5430,7 +5428,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -5463,7 +5461,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'8cpu'!$I$3:$I$10</c:f>
+              <c:f>'8cores'!$I$3:$I$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -5501,7 +5499,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$J$2</c:f>
+              <c:f>'8cores'!$J$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5512,7 +5510,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -5545,7 +5543,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'8cpu'!$J$3:$J$10</c:f>
+              <c:f>'8cores'!$J$3:$J$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -5583,7 +5581,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$K$2</c:f>
+              <c:f>'8cores'!$K$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5594,7 +5592,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -5627,7 +5625,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'8cpu'!$K$3:$K$10</c:f>
+              <c:f>'8cores'!$K$3:$K$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -5665,7 +5663,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$L$2</c:f>
+              <c:f>'8cores'!$L$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5676,7 +5674,7 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -5709,7 +5707,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'8cpu'!$L$3:$L$10</c:f>
+              <c:f>'8cores'!$L$3:$L$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -5747,7 +5745,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$M$2</c:f>
+              <c:f>'8cores'!$M$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5763,7 +5761,7 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -5796,7 +5794,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'8cpu'!$M$3:$M$10</c:f>
+              <c:f>'8cores'!$M$3:$M$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -5834,7 +5832,7 @@
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$N$2</c:f>
+              <c:f>'8cores'!$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5850,7 +5848,7 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -5883,7 +5881,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'8cpu'!$N$3:$N$10</c:f>
+              <c:f>'8cores'!$N$3:$N$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -5921,7 +5919,7 @@
           <c:order val="10"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$O$2</c:f>
+              <c:f>'8cores'!$O$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5937,7 +5935,7 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -5970,7 +5968,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'8cpu'!$O$3:$O$10</c:f>
+              <c:f>'8cores'!$O$3:$O$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -6008,7 +6006,7 @@
           <c:order val="11"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$P$2</c:f>
+              <c:f>'8cores'!$P$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6024,7 +6022,7 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -6057,7 +6055,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'8cpu'!$P$3:$P$10</c:f>
+              <c:f>'8cores'!$P$3:$P$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -6095,7 +6093,7 @@
           <c:order val="12"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$Q$2</c:f>
+              <c:f>'8cores'!$Q$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6111,7 +6109,7 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -6144,7 +6142,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'8cpu'!$Q$3:$Q$10</c:f>
+              <c:f>'8cores'!$Q$3:$Q$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -6182,7 +6180,7 @@
           <c:order val="13"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$R$2</c:f>
+              <c:f>'8cores'!$R$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6198,7 +6196,7 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -6231,7 +6229,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'8cpu'!$R$3:$R$10</c:f>
+              <c:f>'8cores'!$R$3:$R$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -6269,7 +6267,7 @@
           <c:order val="14"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$S$2</c:f>
+              <c:f>'8cores'!$S$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6285,7 +6283,7 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -6318,7 +6316,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'8cpu'!$S$3:$S$10</c:f>
+              <c:f>'8cores'!$S$3:$S$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -6356,7 +6354,7 @@
           <c:order val="15"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$T$2</c:f>
+              <c:f>'8cores'!$T$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6372,7 +6370,7 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -6405,7 +6403,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'8cpu'!$T$3:$T$10</c:f>
+              <c:f>'8cores'!$T$3:$T$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -6443,7 +6441,7 @@
           <c:order val="16"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$U$2</c:f>
+              <c:f>'8cores'!$U$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6459,7 +6457,7 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -6492,7 +6490,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'8cpu'!$U$3:$U$10</c:f>
+              <c:f>'8cores'!$U$3:$U$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -6530,7 +6528,7 @@
           <c:order val="17"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$V$2</c:f>
+              <c:f>'8cores'!$V$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6546,7 +6544,7 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -6579,7 +6577,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'8cpu'!$V$3:$V$10</c:f>
+              <c:f>'8cores'!$V$3:$V$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -6617,7 +6615,7 @@
           <c:order val="18"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$W$2</c:f>
+              <c:f>'8cores'!$W$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6633,7 +6631,7 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -6666,7 +6664,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'8cpu'!$W$3:$W$10</c:f>
+              <c:f>'8cores'!$W$3:$W$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -6704,7 +6702,7 @@
           <c:order val="19"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$X$2</c:f>
+              <c:f>'8cores'!$X$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6720,7 +6718,7 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -6753,7 +6751,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'8cpu'!$X$3:$X$10</c:f>
+              <c:f>'8cores'!$X$3:$X$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -6791,7 +6789,7 @@
           <c:order val="20"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$Y$2</c:f>
+              <c:f>'8cores'!$Y$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6807,7 +6805,7 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -6840,7 +6838,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'8cpu'!$Y$3:$Y$10</c:f>
+              <c:f>'8cores'!$Y$3:$Y$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -6878,7 +6876,7 @@
           <c:order val="21"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$Z$2</c:f>
+              <c:f>'8cores'!$Z$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6894,7 +6892,7 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -6927,7 +6925,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'8cpu'!$Z$3:$Z$10</c:f>
+              <c:f>'8cores'!$Z$3:$Z$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -6965,7 +6963,7 @@
           <c:order val="22"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$AA$2</c:f>
+              <c:f>'8cores'!$AA$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6981,7 +6979,7 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -7014,7 +7012,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'8cpu'!$AA$3:$AA$10</c:f>
+              <c:f>'8cores'!$AA$3:$AA$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -7052,7 +7050,7 @@
           <c:order val="23"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$AB$2</c:f>
+              <c:f>'8cores'!$AB$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7068,7 +7066,7 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -7101,7 +7099,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'8cpu'!$AB$3:$AB$10</c:f>
+              <c:f>'8cores'!$AB$3:$AB$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -7139,7 +7137,7 @@
           <c:order val="24"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$AC$2</c:f>
+              <c:f>'8cores'!$AC$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7155,7 +7153,7 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -7188,7 +7186,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'8cpu'!$AC$3:$AC$10</c:f>
+              <c:f>'8cores'!$AC$3:$AC$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -7229,12 +7227,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="172203008"/>
-        <c:axId val="214474752"/>
-        <c:axId val="214557312"/>
+        <c:axId val="175074304"/>
+        <c:axId val="214170368"/>
+        <c:axId val="214393472"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="172203008"/>
+        <c:axId val="175074304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7270,7 +7268,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="214474752"/>
+        <c:crossAx val="214170368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7278,7 +7276,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="214474752"/>
+        <c:axId val="214170368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7319,12 +7317,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="172203008"/>
+        <c:crossAx val="175074304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="214557312"/>
+        <c:axId val="214393472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7359,7 +7357,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="214474752"/>
+        <c:crossAx val="214170368"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -7410,7 +7408,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -7434,7 +7431,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$E$2</c:f>
+              <c:f>'8cores'!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7445,7 +7442,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -7478,7 +7475,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'8cpu'!$E$3:$E$10</c:f>
+              <c:f>'8cores'!$E$3:$E$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -7516,7 +7513,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$F$2</c:f>
+              <c:f>'8cores'!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7527,7 +7524,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -7560,7 +7557,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'8cpu'!$F$3:$F$10</c:f>
+              <c:f>'8cores'!$F$3:$F$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -7598,7 +7595,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$G$2</c:f>
+              <c:f>'8cores'!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7609,7 +7606,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -7642,7 +7639,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'8cpu'!$G$3:$G$10</c:f>
+              <c:f>'8cores'!$G$3:$G$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -7680,7 +7677,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$H$2</c:f>
+              <c:f>'8cores'!$H$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7691,7 +7688,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -7724,7 +7721,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'8cpu'!$H$3:$H$10</c:f>
+              <c:f>'8cores'!$H$3:$H$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -7762,7 +7759,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$I$2</c:f>
+              <c:f>'8cores'!$I$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7773,7 +7770,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -7806,7 +7803,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'8cpu'!$I$3:$I$10</c:f>
+              <c:f>'8cores'!$I$3:$I$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -7844,7 +7841,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$J$2</c:f>
+              <c:f>'8cores'!$J$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7855,7 +7852,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -7888,7 +7885,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'8cpu'!$J$3:$J$10</c:f>
+              <c:f>'8cores'!$J$3:$J$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -7926,7 +7923,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$K$2</c:f>
+              <c:f>'8cores'!$K$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7937,7 +7934,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -7970,7 +7967,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'8cpu'!$K$3:$K$10</c:f>
+              <c:f>'8cores'!$K$3:$K$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -8008,7 +8005,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$L$2</c:f>
+              <c:f>'8cores'!$L$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8019,7 +8016,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -8052,7 +8049,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'8cpu'!$L$3:$L$10</c:f>
+              <c:f>'8cores'!$L$3:$L$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -8090,7 +8087,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$M$2</c:f>
+              <c:f>'8cores'!$M$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8101,7 +8098,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -8134,7 +8131,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'8cpu'!$M$3:$M$10</c:f>
+              <c:f>'8cores'!$M$3:$M$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -8172,7 +8169,7 @@
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$N$2</c:f>
+              <c:f>'8cores'!$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8183,7 +8180,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -8216,7 +8213,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'8cpu'!$N$3:$N$10</c:f>
+              <c:f>'8cores'!$N$3:$N$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -8254,7 +8251,7 @@
           <c:order val="10"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$O$2</c:f>
+              <c:f>'8cores'!$O$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8265,7 +8262,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -8298,7 +8295,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'8cpu'!$O$3:$O$10</c:f>
+              <c:f>'8cores'!$O$3:$O$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -8336,7 +8333,7 @@
           <c:order val="11"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$P$2</c:f>
+              <c:f>'8cores'!$P$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8347,7 +8344,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -8380,7 +8377,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'8cpu'!$P$3:$P$10</c:f>
+              <c:f>'8cores'!$P$3:$P$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -8418,7 +8415,7 @@
           <c:order val="12"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$Q$2</c:f>
+              <c:f>'8cores'!$Q$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8429,7 +8426,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -8462,7 +8459,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'8cpu'!$Q$3:$Q$10</c:f>
+              <c:f>'8cores'!$Q$3:$Q$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -8500,7 +8497,7 @@
           <c:order val="13"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$R$2</c:f>
+              <c:f>'8cores'!$R$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8511,7 +8508,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -8544,7 +8541,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'8cpu'!$R$3:$R$10</c:f>
+              <c:f>'8cores'!$R$3:$R$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -8582,7 +8579,7 @@
           <c:order val="14"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$S$2</c:f>
+              <c:f>'8cores'!$S$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8593,7 +8590,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -8626,7 +8623,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'8cpu'!$S$3:$S$10</c:f>
+              <c:f>'8cores'!$S$3:$S$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -8664,7 +8661,7 @@
           <c:order val="15"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$T$2</c:f>
+              <c:f>'8cores'!$T$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8675,7 +8672,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -8708,7 +8705,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'8cpu'!$T$3:$T$10</c:f>
+              <c:f>'8cores'!$T$3:$T$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -8746,7 +8743,7 @@
           <c:order val="16"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$U$2</c:f>
+              <c:f>'8cores'!$U$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8757,7 +8754,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -8790,7 +8787,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'8cpu'!$U$3:$U$10</c:f>
+              <c:f>'8cores'!$U$3:$U$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -8828,7 +8825,7 @@
           <c:order val="17"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$V$2</c:f>
+              <c:f>'8cores'!$V$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8839,7 +8836,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -8872,7 +8869,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'8cpu'!$V$3:$V$10</c:f>
+              <c:f>'8cores'!$V$3:$V$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -8910,7 +8907,7 @@
           <c:order val="18"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$W$2</c:f>
+              <c:f>'8cores'!$W$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8921,7 +8918,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -8954,7 +8951,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'8cpu'!$W$3:$W$10</c:f>
+              <c:f>'8cores'!$W$3:$W$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -8992,7 +8989,7 @@
           <c:order val="19"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$X$2</c:f>
+              <c:f>'8cores'!$X$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -9003,7 +9000,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -9036,7 +9033,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'8cpu'!$X$3:$X$10</c:f>
+              <c:f>'8cores'!$X$3:$X$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -9074,7 +9071,7 @@
           <c:order val="20"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$Y$2</c:f>
+              <c:f>'8cores'!$Y$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -9085,7 +9082,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -9118,7 +9115,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'8cpu'!$Y$3:$Y$10</c:f>
+              <c:f>'8cores'!$Y$3:$Y$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -9156,7 +9153,7 @@
           <c:order val="21"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$Z$2</c:f>
+              <c:f>'8cores'!$Z$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -9167,7 +9164,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -9200,7 +9197,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'8cpu'!$Z$3:$Z$10</c:f>
+              <c:f>'8cores'!$Z$3:$Z$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -9238,7 +9235,7 @@
           <c:order val="22"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$AA$2</c:f>
+              <c:f>'8cores'!$AA$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -9249,7 +9246,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -9282,7 +9279,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'8cpu'!$AA$3:$AA$10</c:f>
+              <c:f>'8cores'!$AA$3:$AA$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -9320,7 +9317,7 @@
           <c:order val="23"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$AB$2</c:f>
+              <c:f>'8cores'!$AB$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -9331,7 +9328,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -9364,7 +9361,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'8cpu'!$AB$3:$AB$10</c:f>
+              <c:f>'8cores'!$AB$3:$AB$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -9402,7 +9399,7 @@
           <c:order val="24"/>
           <c:tx>
             <c:strRef>
-              <c:f>'8cpu'!$AC$2</c:f>
+              <c:f>'8cores'!$AC$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -9413,7 +9410,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'8cpu'!$D$3:$D$10</c:f>
+              <c:f>'8cores'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -9446,7 +9443,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'8cpu'!$AC$3:$AC$10</c:f>
+              <c:f>'8cores'!$AC$3:$AC$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -9487,11 +9484,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="240510656"/>
-        <c:axId val="214820544"/>
+        <c:axId val="214681280"/>
+        <c:axId val="214681856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="240510656"/>
+        <c:axId val="214681280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="32"/>
@@ -9529,12 +9526,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="214820544"/>
+        <c:crossAx val="214681856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="214820544"/>
+        <c:axId val="214681856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="55"/>
@@ -9577,7 +9574,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="240510656"/>
+        <c:crossAx val="214681280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9719,11 +9716,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="213209088"/>
-        <c:axId val="214477632"/>
+        <c:axId val="213981184"/>
+        <c:axId val="214683584"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="213209088"/>
+        <c:axId val="213981184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9752,7 +9749,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="214477632"/>
+        <c:crossAx val="214683584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9760,7 +9757,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="214477632"/>
+        <c:axId val="214683584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9790,7 +9787,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="213209088"/>
+        <c:crossAx val="213981184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10368,7 +10365,7 @@
   <dimension ref="A1:F373"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D9"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17768,7 +17765,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Graphs for MPI_OMP 1 & 2 cores
</commit_message>
<xml_diff>
--- a/project-2/results/spreadsheet/openmpi.xlsx
+++ b/project-2/results/spreadsheet/openmpi.xlsx
@@ -861,11 +861,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="212910080"/>
-        <c:axId val="212910656"/>
+        <c:axId val="213177408"/>
+        <c:axId val="213177984"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="212910080"/>
+        <c:axId val="213177408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="32"/>
@@ -896,12 +896,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="212910656"/>
+        <c:crossAx val="213177984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="212910656"/>
+        <c:axId val="213177984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="18"/>
@@ -932,7 +932,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="212910080"/>
+        <c:crossAx val="213177408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -984,6 +984,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1599,12 +1600,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="213980160"/>
-        <c:axId val="212912384"/>
-        <c:axId val="212935936"/>
+        <c:axId val="216982528"/>
+        <c:axId val="213179712"/>
+        <c:axId val="217444992"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="213980160"/>
+        <c:axId val="216982528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1640,7 +1641,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="212912384"/>
+        <c:crossAx val="213179712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1648,7 +1649,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="212912384"/>
+        <c:axId val="213179712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1685,12 +1686,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="213980160"/>
+        <c:crossAx val="216982528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="212935936"/>
+        <c:axId val="217444992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1725,7 +1726,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="212912384"/>
+        <c:crossAx val="213179712"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -1776,6 +1777,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2376,11 +2378,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="212914688"/>
-        <c:axId val="212915264"/>
+        <c:axId val="216901312"/>
+        <c:axId val="216901888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="212914688"/>
+        <c:axId val="216901312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="32"/>
@@ -2418,12 +2420,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="212915264"/>
+        <c:crossAx val="216901888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="212915264"/>
+        <c:axId val="216901888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2460,7 +2462,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="212914688"/>
+        <c:crossAx val="216901312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2512,6 +2514,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3644,12 +3647,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="214294528"/>
-        <c:axId val="212917568"/>
-        <c:axId val="212937216"/>
+        <c:axId val="217935872"/>
+        <c:axId val="216904192"/>
+        <c:axId val="217446272"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="214294528"/>
+        <c:axId val="217935872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3685,7 +3688,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="212917568"/>
+        <c:crossAx val="216904192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3693,7 +3696,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="212917568"/>
+        <c:axId val="216904192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3730,12 +3733,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="214294528"/>
+        <c:crossAx val="217935872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="212937216"/>
+        <c:axId val="217446272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3770,7 +3773,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="212917568"/>
+        <c:crossAx val="216904192"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -3821,6 +3824,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4913,11 +4917,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="214166336"/>
-        <c:axId val="214166912"/>
+        <c:axId val="218038272"/>
+        <c:axId val="218038848"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="214166336"/>
+        <c:axId val="218038272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="32"/>
@@ -4955,12 +4959,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="214166912"/>
+        <c:crossAx val="218038848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="214166912"/>
+        <c:axId val="218038848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="47"/>
@@ -4999,7 +5003,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="214166336"/>
+        <c:crossAx val="218038272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5051,6 +5055,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -7227,12 +7232,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="175074304"/>
-        <c:axId val="214170368"/>
-        <c:axId val="214393472"/>
+        <c:axId val="216981504"/>
+        <c:axId val="218042304"/>
+        <c:axId val="217444352"/>
       </c:line3DChart>
       <c:catAx>
-        <c:axId val="175074304"/>
+        <c:axId val="216981504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7268,7 +7273,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="214170368"/>
+        <c:crossAx val="218042304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7276,7 +7281,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="214170368"/>
+        <c:axId val="218042304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7317,12 +7322,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="175074304"/>
+        <c:crossAx val="216981504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="214393472"/>
+        <c:axId val="217444352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7357,7 +7362,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="214170368"/>
+        <c:crossAx val="218042304"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -7408,6 +7413,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -9484,11 +9490,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="214681280"/>
-        <c:axId val="214681856"/>
+        <c:axId val="218044608"/>
+        <c:axId val="218045184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="214681280"/>
+        <c:axId val="218044608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="32"/>
@@ -9526,12 +9532,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="214681856"/>
+        <c:crossAx val="218045184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="214681856"/>
+        <c:axId val="218045184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="55"/>
@@ -9574,7 +9580,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="214681280"/>
+        <c:crossAx val="218044608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9716,11 +9722,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="213981184"/>
-        <c:axId val="214683584"/>
+        <c:axId val="218375680"/>
+        <c:axId val="218694208"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="213981184"/>
+        <c:axId val="218375680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9749,7 +9755,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="214683584"/>
+        <c:crossAx val="218694208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9757,7 +9763,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="214683584"/>
+        <c:axId val="218694208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9787,7 +9793,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="213981184"/>
+        <c:crossAx val="218375680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17765,7 +17771,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17964,8 +17970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>